<commit_message>
Online-Shop Gantt mit Meilensteinen
</commit_message>
<xml_diff>
--- a/FISIB_Übungen/Online_Shop.Projekt.xlsx
+++ b/FISIB_Übungen/Online_Shop.Projekt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captiva\git\QM_PM\FIAED Übungen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captiva\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8226ABB3-9744-4F4E-985D-0B5E09A773D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA06086-619B-4289-B095-81BE22BC818E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="89">
   <si>
     <t>Beispiel: Funktionsorientierter Projektstrukturplan</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>2. Weihnachtsfeiertag</t>
+  </si>
+  <si>
+    <t>Datenbank vorbereitet</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -776,6 +779,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -783,7 +795,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -977,78 +989,81 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Gantt-Balken" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1059,14 +1074,14 @@
   <dxfs count="31">
     <dxf>
       <font>
-        <color rgb="FFFFBF00"/>
+        <color theme="0"/>
         <name val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFBF00"/>
+          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1095,30 +1110,24 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
         <name val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
+          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1147,30 +1156,11 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+        <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFBF00"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBF00"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1189,43 +1179,47 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
         <name val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFCC0000"/>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFFBF00"/>
+        <color theme="0"/>
         <name val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFBF00"/>
+          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFFFFFF"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+        <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF666666"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1726,6 +1720,191 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>81643</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>210910</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>156483</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Raute 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{984F8099-F3C0-480B-FA43-EB83302ED148}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7497536" y="1694090"/>
+          <a:ext cx="129267" cy="156482"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>102053</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>231320</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>156483</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Raute 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD7067F1-A3EA-4302-ADE0-146FF6BC1FFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10851696" y="2837090"/>
+          <a:ext cx="129267" cy="156482"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>68035</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>149677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>197302</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Raute 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4B3ACD4-8FD7-43C2-B0FB-F7A65F8D2D7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12960803" y="3313338"/>
+          <a:ext cx="129267" cy="156482"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -2035,20 +2214,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="86" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="87"/>
+      <c r="I1" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="80"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -2088,20 +2267,20 @@
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="24.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F5" s="88" t="s">
+      <c r="F5" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="89"/>
+      <c r="G5" s="82"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="90" t="s">
+      <c r="I5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="91"/>
+      <c r="J5" s="84"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="92" t="s">
+      <c r="L5" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="93"/>
+      <c r="M5" s="86"/>
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F6" s="42" t="s">
@@ -2131,18 +2310,18 @@
       <c r="L7" s="36"/>
     </row>
     <row r="8" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="I8" s="77" t="s">
+      <c r="G8" s="88"/>
+      <c r="I8" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="78"/>
-      <c r="L8" s="83" t="s">
+      <c r="J8" s="90"/>
+      <c r="L8" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="84"/>
+      <c r="M8" s="92"/>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F9" s="44" t="s">
@@ -2170,18 +2349,18 @@
       <c r="L10" s="36"/>
     </row>
     <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="81" t="s">
+      <c r="F11" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="82"/>
-      <c r="I11" s="77" t="s">
+      <c r="G11" s="88"/>
+      <c r="I11" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="78"/>
-      <c r="L11" s="83" t="s">
+      <c r="J11" s="90"/>
+      <c r="L11" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="84"/>
+      <c r="M11" s="92"/>
     </row>
     <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F12" s="44" t="s">
@@ -2209,18 +2388,18 @@
       <c r="L13" s="36"/>
     </row>
     <row r="14" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="81" t="s">
+      <c r="F14" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="82"/>
-      <c r="I14" s="77" t="s">
+      <c r="G14" s="88"/>
+      <c r="I14" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="78"/>
-      <c r="L14" s="83" t="s">
+      <c r="J14" s="90"/>
+      <c r="L14" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="M14" s="84"/>
+      <c r="M14" s="92"/>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F15" s="44" t="s">
@@ -2247,14 +2426,14 @@
       <c r="I16" s="36"/>
     </row>
     <row r="17" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F17" s="81" t="s">
+      <c r="F17" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="82"/>
-      <c r="I17" s="77" t="s">
+      <c r="G17" s="88"/>
+      <c r="I17" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="78"/>
+      <c r="J17" s="90"/>
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F18" s="44" t="s">
@@ -2274,10 +2453,10 @@
       <c r="I19" s="36"/>
     </row>
     <row r="20" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I20" s="77" t="s">
+      <c r="I20" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="78"/>
+      <c r="J20" s="90"/>
     </row>
     <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I21" s="48" t="s">
@@ -2291,10 +2470,10 @@
       <c r="I22" s="36"/>
     </row>
     <row r="23" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I23" s="77" t="s">
+      <c r="I23" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="J23" s="78"/>
+      <c r="J23" s="90"/>
     </row>
     <row r="24" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I24" s="48" t="s">
@@ -2308,11 +2487,11 @@
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="79" t="s">
+      <c r="B25" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="I25" s="36"/>
@@ -2321,27 +2500,27 @@
       <c r="A26" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="80" t="s">
+      <c r="B26" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
-      <c r="I26" s="77" t="s">
+      <c r="I26" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="J26" s="78"/>
+      <c r="J26" s="90"/>
     </row>
     <row r="27" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="75" t="s">
+      <c r="B27" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="I27" s="48" t="s">
@@ -2355,11 +2534,11 @@
       <c r="A28" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="75" t="s">
+      <c r="B28" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="95"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="I28" s="36"/>
@@ -2368,27 +2547,27 @@
       <c r="A29" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="75" t="s">
+      <c r="B29" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
-      <c r="I29" s="77" t="s">
+      <c r="I29" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="J29" s="78"/>
+      <c r="J29" s="90"/>
     </row>
     <row r="30" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="75" t="s">
+      <c r="B30" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="95"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="I30" s="48" t="s">
@@ -2402,11 +2581,11 @@
       <c r="A31" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="75" t="s">
+      <c r="B31" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="95"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="I31" s="36"/>
@@ -2415,27 +2594,27 @@
       <c r="A32" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="75" t="s">
+      <c r="B32" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="95"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="I32" s="77" t="s">
+      <c r="I32" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="J32" s="78"/>
+      <c r="J32" s="90"/>
     </row>
     <row r="33" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="75" t="s">
+      <c r="B33" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="95"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="I33" s="48" t="s">
@@ -2449,11 +2628,11 @@
       <c r="A34" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="75" t="s">
+      <c r="B34" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
@@ -2461,11 +2640,11 @@
       <c r="A35" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="75" t="s">
+      <c r="B35" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="75"/>
-      <c r="D35" s="75"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="95"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
@@ -2473,11 +2652,11 @@
       <c r="A36" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="75" t="s">
+      <c r="B36" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="75"/>
-      <c r="D36" s="75"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="95"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
@@ -2485,11 +2664,11 @@
       <c r="A37" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="75" t="s">
+      <c r="B37" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="95"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
@@ -2497,11 +2676,11 @@
       <c r="A38" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="75" t="s">
+      <c r="B38" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="75"/>
-      <c r="D38" s="75"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="95"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
@@ -2509,11 +2688,11 @@
       <c r="A39" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="75" t="s">
+      <c r="B39" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="75"/>
-      <c r="D39" s="75"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="95"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
@@ -2521,11 +2700,11 @@
       <c r="A40" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="75" t="s">
+      <c r="B40" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="75"/>
-      <c r="D40" s="75"/>
+      <c r="C40" s="95"/>
+      <c r="D40" s="95"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
@@ -2533,47 +2712,16 @@
       <c r="A41" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="76" t="s">
+      <c r="B41" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="96"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B35:D35"/>
@@ -2581,6 +2729,37 @@
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="L5:M5"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2595,8 +2774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BQ23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="AA1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3:AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7109375" defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2613,11 +2792,11 @@
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
       <c r="E1" s="14" t="s">
         <v>46</v>
       </c>
@@ -2641,11 +2820,11 @@
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
       <c r="E2" s="16"/>
       <c r="F2" s="17" t="s">
         <v>52</v>
@@ -2766,11 +2945,11 @@
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
       <c r="E3" s="20" t="s">
         <v>16</v>
       </c>
@@ -2790,25 +2969,25 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L3" s="94" t="s">
+      <c r="L3" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
       <c r="O3" s="54"/>
       <c r="P3" s="55"/>
-      <c r="Q3" s="94" t="s">
+      <c r="Q3" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="94"/>
-      <c r="S3" s="94"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="97"/>
       <c r="T3" s="54"/>
       <c r="U3" s="55"/>
-      <c r="V3" s="94" t="s">
+      <c r="V3" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="W3" s="94"/>
-      <c r="X3" s="94"/>
+      <c r="W3" s="97"/>
+      <c r="X3" s="97"/>
       <c r="Y3" s="54"/>
       <c r="Z3" s="59"/>
       <c r="AA3" s="59"/>
@@ -2816,70 +2995,70 @@
       <c r="AC3" s="59"/>
       <c r="AD3" s="59"/>
       <c r="AE3" s="55"/>
-      <c r="AF3" s="94" t="s">
+      <c r="AF3" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" s="94"/>
-      <c r="AH3" s="94"/>
+      <c r="AG3" s="97"/>
+      <c r="AH3" s="97"/>
       <c r="AI3" s="54"/>
       <c r="AJ3" s="55"/>
-      <c r="AK3" s="94" t="s">
+      <c r="AK3" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="AL3" s="94"/>
-      <c r="AM3" s="94"/>
+      <c r="AL3" s="97"/>
+      <c r="AM3" s="97"/>
       <c r="AN3" s="54"/>
       <c r="AO3" s="55"/>
-      <c r="AP3" s="94" t="s">
+      <c r="AP3" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="AQ3" s="94"/>
-      <c r="AR3" s="94"/>
+      <c r="AQ3" s="97"/>
+      <c r="AR3" s="97"/>
       <c r="AS3" s="54"/>
       <c r="AT3" s="55"/>
-      <c r="AU3" s="94" t="s">
+      <c r="AU3" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="AV3" s="94"/>
-      <c r="AW3" s="94"/>
+      <c r="AV3" s="97"/>
+      <c r="AW3" s="97"/>
       <c r="AX3" s="54"/>
       <c r="AY3" s="55"/>
-      <c r="AZ3" s="94" t="s">
+      <c r="AZ3" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="BA3" s="94"/>
-      <c r="BB3" s="94"/>
+      <c r="BA3" s="97"/>
+      <c r="BB3" s="97"/>
       <c r="BC3" s="54"/>
       <c r="BD3" s="55"/>
-      <c r="BE3" s="94" t="s">
+      <c r="BE3" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="BF3" s="94"/>
-      <c r="BG3" s="94"/>
+      <c r="BF3" s="97"/>
+      <c r="BG3" s="97"/>
       <c r="BH3" s="54"/>
       <c r="BI3" s="55"/>
-      <c r="BJ3" s="94" t="s">
+      <c r="BJ3" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="BK3" s="94"/>
-      <c r="BL3" s="94"/>
+      <c r="BK3" s="97"/>
+      <c r="BL3" s="97"/>
       <c r="BM3" s="54"/>
       <c r="BN3" s="55"/>
-      <c r="BO3" s="94" t="s">
+      <c r="BO3" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="BP3" s="94"/>
-      <c r="BQ3" s="94"/>
+      <c r="BP3" s="97"/>
+      <c r="BQ3" s="97"/>
     </row>
     <row r="4" spans="1:69" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
       <c r="E4" s="20" t="s">
         <v>15</v>
       </c>
@@ -3037,11 +3216,11 @@
       <c r="A5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
       <c r="E5" s="20" t="s">
         <v>15</v>
       </c>
@@ -3170,11 +3349,11 @@
       <c r="A6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
       <c r="E6" s="23" t="s">
         <v>27</v>
       </c>
@@ -3205,11 +3384,11 @@
       <c r="A7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
       <c r="E7" s="20" t="s">
         <v>16</v>
       </c>
@@ -3239,11 +3418,11 @@
       <c r="A8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
       <c r="E8" s="23" t="s">
         <v>22</v>
       </c>
@@ -3291,11 +3470,11 @@
       <c r="A9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="95"/>
       <c r="E9" s="23" t="s">
         <v>56</v>
       </c>
@@ -3318,18 +3497,18 @@
       </c>
       <c r="O9" s="56"/>
       <c r="T9" s="56"/>
-      <c r="V9" s="94" t="s">
+      <c r="V9" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="W9" s="94"/>
-      <c r="X9" s="94"/>
+      <c r="W9" s="97"/>
+      <c r="X9" s="97"/>
       <c r="Y9" s="54"/>
       <c r="Z9" s="55"/>
-      <c r="AA9" s="94" t="s">
+      <c r="AA9" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="AB9" s="94"/>
-      <c r="AC9" s="94"/>
+      <c r="AB9" s="97"/>
+      <c r="AC9" s="97"/>
       <c r="AD9" s="60"/>
       <c r="AE9" s="56"/>
       <c r="BM9" s="56"/>
@@ -3338,11 +3517,11 @@
       <c r="A10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
       <c r="E10" s="23" t="s">
         <v>33</v>
       </c>
@@ -3396,11 +3575,11 @@
       <c r="A11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="95"/>
       <c r="E11" s="23" t="s">
         <v>35</v>
       </c>
@@ -3447,11 +3626,11 @@
       <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
       <c r="E12" s="23" t="s">
         <v>28</v>
       </c>
@@ -3484,11 +3663,11 @@
       <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
       <c r="E13" s="23" t="s">
         <v>37</v>
       </c>
@@ -3517,11 +3696,11 @@
       <c r="A14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
       <c r="E14" s="23" t="s">
         <v>23</v>
       </c>
@@ -3577,11 +3756,11 @@
       <c r="A15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
       <c r="E15" s="23" t="s">
         <v>41</v>
       </c>
@@ -3604,25 +3783,25 @@
       </c>
       <c r="O15" s="56"/>
       <c r="P15" s="57"/>
-      <c r="Q15" s="94" t="s">
+      <c r="Q15" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="R15" s="94"/>
-      <c r="S15" s="94"/>
+      <c r="R15" s="97"/>
+      <c r="S15" s="97"/>
       <c r="T15" s="54"/>
       <c r="U15" s="55"/>
-      <c r="V15" s="94" t="s">
+      <c r="V15" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="W15" s="94"/>
-      <c r="X15" s="94"/>
+      <c r="W15" s="97"/>
+      <c r="X15" s="97"/>
       <c r="Y15" s="54"/>
       <c r="Z15" s="55"/>
-      <c r="AA15" s="94" t="s">
+      <c r="AA15" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="AB15" s="94"/>
-      <c r="AC15" s="94"/>
+      <c r="AB15" s="97"/>
+      <c r="AC15" s="97"/>
       <c r="AD15" s="54"/>
       <c r="AE15" s="59"/>
       <c r="AF15" s="59"/>
@@ -3664,11 +3843,11 @@
       <c r="A16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
       <c r="E16" s="23" t="s">
         <v>29</v>
       </c>
@@ -3730,11 +3909,11 @@
       <c r="A17" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="76" t="s">
+      <c r="B17" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
       <c r="E17" s="24" t="s">
         <v>58</v>
       </c>
@@ -3781,9 +3960,9 @@
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="G18" s="95"/>
-      <c r="H18" s="95"/>
-      <c r="I18" s="95"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="71" t="s">
@@ -3806,11 +3985,11 @@
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A21" s="94" t="s">
+      <c r="A21" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="94"/>
-      <c r="C21" s="94"/>
+      <c r="B21" s="97"/>
+      <c r="C21" s="97"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" s="68" t="s">
@@ -3840,11 +4019,26 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="AA15:AC15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="AA9:AC9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="AZ3:BB3"/>
     <mergeCell ref="BE3:BG3"/>
     <mergeCell ref="BJ3:BL3"/>
@@ -3855,26 +4049,11 @@
     <mergeCell ref="AK3:AM3"/>
     <mergeCell ref="AP3:AR3"/>
     <mergeCell ref="AU3:AW3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="AA9:AC9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="V15:X15"/>
-    <mergeCell ref="AA15:AC15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="Q3:S3"/>
   </mergeCells>
   <conditionalFormatting sqref="B22">
     <cfRule type="cellIs" dxfId="30" priority="17" operator="equal">
@@ -3973,11 +4152,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BN17"/>
+  <dimension ref="A1:BN20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="11" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L3" sqref="L3"/>
+      <pane xSplit="11" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BB20" sqref="BB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -3995,11 +4174,11 @@
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
       <c r="E1" s="14" t="s">
         <v>46</v>
       </c>
@@ -4189,11 +4368,11 @@
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
       <c r="E2" s="16"/>
       <c r="F2" s="17" t="s">
         <v>52</v>
@@ -4216,73 +4395,76 @@
       </c>
       <c r="K2" s="31">
         <f t="shared" ref="K2:K8" si="0">SUM(L2:BM2)</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="97"/>
-      <c r="S2" s="97"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="97"/>
-      <c r="V2" s="97"/>
-      <c r="W2" s="97"/>
-      <c r="X2" s="97"/>
-      <c r="Y2" s="97"/>
-      <c r="Z2" s="97"/>
-      <c r="AA2" s="97"/>
-      <c r="AB2" s="97"/>
-      <c r="AC2" s="97"/>
-      <c r="AD2" s="97"/>
-      <c r="AE2" s="97"/>
-      <c r="AF2" s="97"/>
-      <c r="AG2" s="97"/>
-      <c r="AH2" s="97"/>
-      <c r="AI2" s="97"/>
-      <c r="AJ2" s="97"/>
-      <c r="AK2" s="97"/>
-      <c r="AL2" s="97"/>
-      <c r="AM2" s="97"/>
-      <c r="AN2" s="97"/>
-      <c r="AO2" s="97"/>
-      <c r="AP2" s="97"/>
-      <c r="AQ2" s="97"/>
-      <c r="AR2" s="97"/>
-      <c r="AS2" s="97"/>
-      <c r="AT2" s="97"/>
-      <c r="AU2" s="97"/>
-      <c r="AV2" s="97"/>
-      <c r="AW2" s="97"/>
-      <c r="AX2" s="97"/>
-      <c r="AY2" s="98"/>
-      <c r="AZ2" s="97"/>
-      <c r="BA2" s="97"/>
-      <c r="BB2" s="97"/>
-      <c r="BC2" s="97"/>
-      <c r="BD2" s="97"/>
-      <c r="BE2" s="97"/>
-      <c r="BF2" s="98"/>
-      <c r="BG2" s="97"/>
-      <c r="BH2" s="97"/>
-      <c r="BI2" s="97"/>
-      <c r="BJ2" s="97"/>
-      <c r="BK2" s="97"/>
-      <c r="BL2" s="98"/>
-      <c r="BM2" s="97"/>
-      <c r="BN2" s="99"/>
+        <v>2</v>
+      </c>
+      <c r="L2" s="21">
+        <v>1</v>
+      </c>
+      <c r="M2" s="21">
+        <v>1</v>
+      </c>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="10"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="10"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="75"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="10"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="10"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="10"/>
+      <c r="BF2" s="75"/>
+      <c r="BG2" s="10"/>
+      <c r="BH2" s="10"/>
+      <c r="BI2" s="10"/>
+      <c r="BJ2" s="10"/>
+      <c r="BK2" s="10"/>
+      <c r="BL2" s="75"/>
+      <c r="BM2" s="10"/>
     </row>
     <row r="3" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
       <c r="E3" s="20" t="s">
         <v>16</v>
       </c>
@@ -4307,73 +4489,74 @@
       </c>
       <c r="K3" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="96"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
-      <c r="AC3" s="97"/>
-      <c r="AD3" s="97"/>
-      <c r="AE3" s="97"/>
-      <c r="AF3" s="97"/>
-      <c r="AG3" s="97"/>
-      <c r="AH3" s="97"/>
-      <c r="AI3" s="97"/>
-      <c r="AJ3" s="97"/>
-      <c r="AK3" s="97"/>
-      <c r="AL3" s="97"/>
-      <c r="AM3" s="97"/>
-      <c r="AN3" s="97"/>
-      <c r="AO3" s="97"/>
-      <c r="AP3" s="97"/>
-      <c r="AQ3" s="97"/>
-      <c r="AR3" s="97"/>
-      <c r="AS3" s="97"/>
-      <c r="AT3" s="97"/>
-      <c r="AU3" s="97"/>
-      <c r="AV3" s="97"/>
-      <c r="AW3" s="97"/>
-      <c r="AX3" s="97"/>
-      <c r="AY3" s="98"/>
-      <c r="AZ3" s="97"/>
-      <c r="BA3" s="97"/>
-      <c r="BB3" s="97"/>
-      <c r="BC3" s="97"/>
-      <c r="BD3" s="97"/>
-      <c r="BE3" s="97"/>
-      <c r="BF3" s="98"/>
-      <c r="BG3" s="97"/>
-      <c r="BH3" s="97"/>
-      <c r="BI3" s="97"/>
-      <c r="BJ3" s="97"/>
-      <c r="BK3" s="97"/>
-      <c r="BL3" s="98"/>
-      <c r="BM3" s="97"/>
-      <c r="BN3" s="99"/>
+        <v>1</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10">
+        <v>1</v>
+      </c>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="10"/>
+      <c r="AJ3" s="10"/>
+      <c r="AK3" s="10"/>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="10"/>
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="10"/>
+      <c r="AP3" s="10"/>
+      <c r="AQ3" s="10"/>
+      <c r="AR3" s="10"/>
+      <c r="AS3" s="10"/>
+      <c r="AT3" s="10"/>
+      <c r="AU3" s="10"/>
+      <c r="AV3" s="10"/>
+      <c r="AW3" s="10"/>
+      <c r="AX3" s="10"/>
+      <c r="AY3" s="75"/>
+      <c r="AZ3" s="10"/>
+      <c r="BA3" s="10"/>
+      <c r="BB3" s="10"/>
+      <c r="BC3" s="10"/>
+      <c r="BD3" s="10"/>
+      <c r="BE3" s="10"/>
+      <c r="BF3" s="75"/>
+      <c r="BG3" s="10"/>
+      <c r="BH3" s="10"/>
+      <c r="BI3" s="10"/>
+      <c r="BJ3" s="10"/>
+      <c r="BK3" s="10"/>
+      <c r="BL3" s="75"/>
+      <c r="BM3" s="10"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
       <c r="E4" s="20" t="s">
         <v>15</v>
       </c>
@@ -4398,73 +4581,80 @@
       </c>
       <c r="K4" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="97"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="96"/>
-      <c r="U4" s="96"/>
-      <c r="V4" s="96"/>
-      <c r="W4" s="96"/>
-      <c r="X4" s="97"/>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="97"/>
-      <c r="AA4" s="97"/>
-      <c r="AB4" s="97"/>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="97"/>
-      <c r="AE4" s="97"/>
-      <c r="AF4" s="97"/>
-      <c r="AG4" s="97"/>
-      <c r="AH4" s="97"/>
-      <c r="AI4" s="97"/>
-      <c r="AJ4" s="97"/>
-      <c r="AK4" s="97"/>
-      <c r="AL4" s="97"/>
-      <c r="AM4" s="97"/>
-      <c r="AN4" s="97"/>
-      <c r="AO4" s="97"/>
-      <c r="AP4" s="97"/>
-      <c r="AQ4" s="97"/>
-      <c r="AR4" s="97"/>
-      <c r="AS4" s="97"/>
-      <c r="AT4" s="97"/>
-      <c r="AU4" s="97"/>
-      <c r="AV4" s="97"/>
-      <c r="AW4" s="97"/>
-      <c r="AX4" s="97"/>
-      <c r="AY4" s="98"/>
-      <c r="AZ4" s="97"/>
-      <c r="BA4" s="97"/>
-      <c r="BB4" s="97"/>
-      <c r="BC4" s="97"/>
-      <c r="BD4" s="97"/>
-      <c r="BE4" s="97"/>
-      <c r="BF4" s="98"/>
-      <c r="BG4" s="97"/>
-      <c r="BH4" s="97"/>
-      <c r="BI4" s="97"/>
-      <c r="BJ4" s="97"/>
-      <c r="BK4" s="97"/>
-      <c r="BL4" s="98"/>
-      <c r="BM4" s="97"/>
-      <c r="BN4" s="99"/>
+        <v>4</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10">
+        <v>1</v>
+      </c>
+      <c r="P4" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10">
+        <v>1</v>
+      </c>
+      <c r="T4" s="21">
+        <v>1</v>
+      </c>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="10"/>
+      <c r="AH4" s="10"/>
+      <c r="AI4" s="10"/>
+      <c r="AJ4" s="10"/>
+      <c r="AK4" s="10"/>
+      <c r="AL4" s="10"/>
+      <c r="AM4" s="10"/>
+      <c r="AN4" s="10"/>
+      <c r="AO4" s="10"/>
+      <c r="AP4" s="10"/>
+      <c r="AQ4" s="10"/>
+      <c r="AR4" s="10"/>
+      <c r="AS4" s="10"/>
+      <c r="AT4" s="10"/>
+      <c r="AU4" s="10"/>
+      <c r="AV4" s="10"/>
+      <c r="AW4" s="10"/>
+      <c r="AX4" s="10"/>
+      <c r="AY4" s="75"/>
+      <c r="AZ4" s="10"/>
+      <c r="BA4" s="10"/>
+      <c r="BB4" s="10"/>
+      <c r="BC4" s="10"/>
+      <c r="BD4" s="10"/>
+      <c r="BE4" s="10"/>
+      <c r="BF4" s="75"/>
+      <c r="BG4" s="10"/>
+      <c r="BH4" s="10"/>
+      <c r="BI4" s="10"/>
+      <c r="BJ4" s="10"/>
+      <c r="BK4" s="10"/>
+      <c r="BL4" s="75"/>
+      <c r="BM4" s="10"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
       <c r="E5" s="20" t="s">
         <v>15</v>
       </c>
@@ -4489,73 +4679,78 @@
       </c>
       <c r="K5" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
-      <c r="N5" s="97"/>
-      <c r="O5" s="97"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="97"/>
-      <c r="R5" s="97"/>
-      <c r="S5" s="97"/>
-      <c r="T5" s="96"/>
-      <c r="U5" s="96"/>
-      <c r="V5" s="96"/>
-      <c r="W5" s="97"/>
-      <c r="X5" s="97"/>
-      <c r="Y5" s="97"/>
-      <c r="Z5" s="97"/>
-      <c r="AA5" s="97"/>
-      <c r="AB5" s="97"/>
-      <c r="AC5" s="97"/>
-      <c r="AD5" s="97"/>
-      <c r="AE5" s="97"/>
-      <c r="AF5" s="97"/>
-      <c r="AG5" s="97"/>
-      <c r="AH5" s="97"/>
-      <c r="AI5" s="97"/>
-      <c r="AJ5" s="97"/>
-      <c r="AK5" s="97"/>
-      <c r="AL5" s="97"/>
-      <c r="AM5" s="97"/>
-      <c r="AN5" s="97"/>
-      <c r="AO5" s="97"/>
-      <c r="AP5" s="97"/>
-      <c r="AQ5" s="97"/>
-      <c r="AR5" s="97"/>
-      <c r="AS5" s="97"/>
-      <c r="AT5" s="97"/>
-      <c r="AU5" s="97"/>
-      <c r="AV5" s="97"/>
-      <c r="AW5" s="97"/>
-      <c r="AX5" s="97"/>
-      <c r="AY5" s="98"/>
-      <c r="AZ5" s="97"/>
-      <c r="BA5" s="97"/>
-      <c r="BB5" s="97"/>
-      <c r="BC5" s="97"/>
-      <c r="BD5" s="97"/>
-      <c r="BE5" s="97"/>
-      <c r="BF5" s="98"/>
-      <c r="BG5" s="97"/>
-      <c r="BH5" s="97"/>
-      <c r="BI5" s="97"/>
-      <c r="BJ5" s="97"/>
-      <c r="BK5" s="97"/>
-      <c r="BL5" s="98"/>
-      <c r="BM5" s="97"/>
-      <c r="BN5" s="99"/>
+        <v>3</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10">
+        <v>1</v>
+      </c>
+      <c r="P5" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10">
+        <v>1</v>
+      </c>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="10"/>
+      <c r="AL5" s="10"/>
+      <c r="AM5" s="10"/>
+      <c r="AN5" s="10"/>
+      <c r="AO5" s="10"/>
+      <c r="AP5" s="10"/>
+      <c r="AQ5" s="10"/>
+      <c r="AR5" s="10"/>
+      <c r="AS5" s="10"/>
+      <c r="AT5" s="10"/>
+      <c r="AU5" s="10"/>
+      <c r="AV5" s="10"/>
+      <c r="AW5" s="10"/>
+      <c r="AX5" s="10"/>
+      <c r="AY5" s="75"/>
+      <c r="AZ5" s="10"/>
+      <c r="BA5" s="10"/>
+      <c r="BB5" s="10"/>
+      <c r="BC5" s="10"/>
+      <c r="BD5" s="10"/>
+      <c r="BE5" s="10"/>
+      <c r="BF5" s="75"/>
+      <c r="BG5" s="10"/>
+      <c r="BH5" s="10"/>
+      <c r="BI5" s="10"/>
+      <c r="BJ5" s="10"/>
+      <c r="BK5" s="10"/>
+      <c r="BL5" s="75"/>
+      <c r="BM5" s="10"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
       <c r="E6" s="23" t="s">
         <v>27</v>
       </c>
@@ -4580,73 +4775,82 @@
       </c>
       <c r="K6" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L6" s="97"/>
-      <c r="M6" s="97"/>
-      <c r="N6" s="97"/>
-      <c r="O6" s="97"/>
-      <c r="P6" s="97"/>
-      <c r="Q6" s="97"/>
-      <c r="R6" s="97"/>
-      <c r="S6" s="97"/>
-      <c r="T6" s="97"/>
-      <c r="U6" s="97"/>
-      <c r="V6" s="97"/>
-      <c r="W6" s="96"/>
-      <c r="X6" s="97"/>
-      <c r="Y6" s="97"/>
-      <c r="Z6" s="96"/>
-      <c r="AA6" s="96"/>
-      <c r="AB6" s="96"/>
-      <c r="AC6" s="96"/>
-      <c r="AD6" s="97"/>
-      <c r="AE6" s="97"/>
-      <c r="AF6" s="97"/>
-      <c r="AG6" s="97"/>
-      <c r="AH6" s="97"/>
-      <c r="AI6" s="97"/>
-      <c r="AJ6" s="97"/>
-      <c r="AK6" s="97"/>
-      <c r="AL6" s="97"/>
-      <c r="AM6" s="97"/>
-      <c r="AN6" s="97"/>
-      <c r="AO6" s="97"/>
-      <c r="AP6" s="97"/>
-      <c r="AQ6" s="97"/>
-      <c r="AR6" s="97"/>
-      <c r="AS6" s="97"/>
-      <c r="AT6" s="97"/>
-      <c r="AU6" s="97"/>
-      <c r="AV6" s="97"/>
-      <c r="AW6" s="97"/>
-      <c r="AX6" s="97"/>
-      <c r="AY6" s="98"/>
-      <c r="AZ6" s="97"/>
-      <c r="BA6" s="97"/>
-      <c r="BB6" s="97"/>
-      <c r="BC6" s="97"/>
-      <c r="BD6" s="97"/>
-      <c r="BE6" s="97"/>
-      <c r="BF6" s="98"/>
-      <c r="BG6" s="97"/>
-      <c r="BH6" s="97"/>
-      <c r="BI6" s="97"/>
-      <c r="BJ6" s="97"/>
-      <c r="BK6" s="97"/>
-      <c r="BL6" s="98"/>
-      <c r="BM6" s="97"/>
-      <c r="BN6" s="99"/>
+        <v>5</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10">
+        <v>1</v>
+      </c>
+      <c r="U6" s="10">
+        <v>1</v>
+      </c>
+      <c r="V6" s="10">
+        <v>1</v>
+      </c>
+      <c r="W6" s="10">
+        <v>1</v>
+      </c>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="21">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="21"/>
+      <c r="AC6" s="21"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
+      <c r="AM6" s="10"/>
+      <c r="AN6" s="10"/>
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="10"/>
+      <c r="AV6" s="10"/>
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="10"/>
+      <c r="AY6" s="75"/>
+      <c r="AZ6" s="10"/>
+      <c r="BA6" s="10"/>
+      <c r="BB6" s="10"/>
+      <c r="BC6" s="10"/>
+      <c r="BD6" s="10"/>
+      <c r="BE6" s="10"/>
+      <c r="BF6" s="75"/>
+      <c r="BG6" s="10"/>
+      <c r="BH6" s="10"/>
+      <c r="BI6" s="10"/>
+      <c r="BJ6" s="10"/>
+      <c r="BK6" s="10"/>
+      <c r="BL6" s="75"/>
+      <c r="BM6" s="10"/>
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
       <c r="E7" s="20" t="s">
         <v>16</v>
       </c>
@@ -4671,73 +4875,74 @@
       </c>
       <c r="K7" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="97"/>
-      <c r="M7" s="97"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="97"/>
-      <c r="P7" s="97"/>
-      <c r="Q7" s="97"/>
-      <c r="R7" s="97"/>
-      <c r="S7" s="96"/>
-      <c r="T7" s="97"/>
-      <c r="U7" s="97"/>
-      <c r="V7" s="97"/>
-      <c r="W7" s="97"/>
-      <c r="X7" s="97"/>
-      <c r="Y7" s="97"/>
-      <c r="Z7" s="97"/>
-      <c r="AA7" s="97"/>
-      <c r="AB7" s="97"/>
-      <c r="AC7" s="97"/>
-      <c r="AD7" s="97"/>
-      <c r="AE7" s="97"/>
-      <c r="AF7" s="97"/>
-      <c r="AG7" s="97"/>
-      <c r="AH7" s="97"/>
-      <c r="AI7" s="97"/>
-      <c r="AJ7" s="97"/>
-      <c r="AK7" s="97"/>
-      <c r="AL7" s="97"/>
-      <c r="AM7" s="97"/>
-      <c r="AN7" s="97"/>
-      <c r="AO7" s="97"/>
-      <c r="AP7" s="97"/>
-      <c r="AQ7" s="97"/>
-      <c r="AR7" s="97"/>
-      <c r="AS7" s="97"/>
-      <c r="AT7" s="97"/>
-      <c r="AU7" s="97"/>
-      <c r="AV7" s="97"/>
-      <c r="AW7" s="97"/>
-      <c r="AX7" s="97"/>
-      <c r="AY7" s="98"/>
-      <c r="AZ7" s="97"/>
-      <c r="BA7" s="97"/>
-      <c r="BB7" s="97"/>
-      <c r="BC7" s="97"/>
-      <c r="BD7" s="97"/>
-      <c r="BE7" s="97"/>
-      <c r="BF7" s="98"/>
-      <c r="BG7" s="97"/>
-      <c r="BH7" s="97"/>
-      <c r="BI7" s="97"/>
-      <c r="BJ7" s="97"/>
-      <c r="BK7" s="97"/>
-      <c r="BL7" s="98"/>
-      <c r="BM7" s="97"/>
-      <c r="BN7" s="99"/>
+        <v>1</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10">
+        <v>1</v>
+      </c>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="10"/>
+      <c r="AJ7" s="10"/>
+      <c r="AK7" s="10"/>
+      <c r="AL7" s="10"/>
+      <c r="AM7" s="10"/>
+      <c r="AN7" s="10"/>
+      <c r="AO7" s="10"/>
+      <c r="AP7" s="10"/>
+      <c r="AQ7" s="10"/>
+      <c r="AR7" s="10"/>
+      <c r="AS7" s="10"/>
+      <c r="AT7" s="10"/>
+      <c r="AU7" s="10"/>
+      <c r="AV7" s="10"/>
+      <c r="AW7" s="10"/>
+      <c r="AX7" s="10"/>
+      <c r="AY7" s="75"/>
+      <c r="AZ7" s="10"/>
+      <c r="BA7" s="10"/>
+      <c r="BB7" s="10"/>
+      <c r="BC7" s="10"/>
+      <c r="BD7" s="10"/>
+      <c r="BE7" s="10"/>
+      <c r="BF7" s="75"/>
+      <c r="BG7" s="10"/>
+      <c r="BH7" s="10"/>
+      <c r="BI7" s="10"/>
+      <c r="BJ7" s="10"/>
+      <c r="BK7" s="10"/>
+      <c r="BL7" s="75"/>
+      <c r="BM7" s="10"/>
     </row>
     <row r="8" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
       <c r="E8" s="23" t="s">
         <v>22</v>
       </c>
@@ -4762,914 +4967,1185 @@
       </c>
       <c r="K8" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="97"/>
-      <c r="O8" s="97"/>
-      <c r="P8" s="97"/>
-      <c r="Q8" s="97"/>
-      <c r="R8" s="97"/>
-      <c r="S8" s="97"/>
-      <c r="T8" s="96"/>
-      <c r="U8" s="96"/>
-      <c r="V8" s="96"/>
-      <c r="W8" s="97"/>
-      <c r="X8" s="97"/>
-      <c r="Y8" s="97"/>
-      <c r="Z8" s="97"/>
-      <c r="AA8" s="97"/>
-      <c r="AB8" s="97"/>
-      <c r="AC8" s="97"/>
-      <c r="AD8" s="97"/>
-      <c r="AE8" s="97"/>
-      <c r="AF8" s="97"/>
-      <c r="AG8" s="97"/>
-      <c r="AH8" s="97"/>
-      <c r="AI8" s="97"/>
-      <c r="AJ8" s="97"/>
-      <c r="AK8" s="97"/>
-      <c r="AL8" s="97"/>
-      <c r="AM8" s="97"/>
-      <c r="AN8" s="97"/>
-      <c r="AO8" s="97"/>
-      <c r="AP8" s="97"/>
-      <c r="AQ8" s="97"/>
-      <c r="AR8" s="97"/>
-      <c r="AS8" s="97"/>
-      <c r="AT8" s="97"/>
-      <c r="AU8" s="97"/>
-      <c r="AV8" s="97"/>
-      <c r="AW8" s="97"/>
-      <c r="AX8" s="97"/>
-      <c r="AY8" s="98"/>
-      <c r="AZ8" s="97"/>
-      <c r="BA8" s="97"/>
-      <c r="BB8" s="97"/>
-      <c r="BC8" s="97"/>
-      <c r="BD8" s="97"/>
-      <c r="BE8" s="97"/>
-      <c r="BF8" s="98"/>
-      <c r="BG8" s="97"/>
-      <c r="BH8" s="97"/>
-      <c r="BI8" s="97"/>
-      <c r="BJ8" s="97"/>
-      <c r="BK8" s="97"/>
-      <c r="BL8" s="98"/>
-      <c r="BM8" s="97"/>
-      <c r="BN8" s="99"/>
+        <v>4</v>
+      </c>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10">
+        <v>1</v>
+      </c>
+      <c r="P8" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10">
+        <v>1</v>
+      </c>
+      <c r="T8" s="21">
+        <v>1</v>
+      </c>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="10"/>
+      <c r="AJ8" s="10"/>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="10"/>
+      <c r="AM8" s="10"/>
+      <c r="AN8" s="10"/>
+      <c r="AO8" s="10"/>
+      <c r="AP8" s="10"/>
+      <c r="AQ8" s="10"/>
+      <c r="AR8" s="10"/>
+      <c r="AS8" s="10"/>
+      <c r="AT8" s="10"/>
+      <c r="AU8" s="10"/>
+      <c r="AV8" s="10"/>
+      <c r="AW8" s="10"/>
+      <c r="AX8" s="10"/>
+      <c r="AY8" s="75"/>
+      <c r="AZ8" s="10"/>
+      <c r="BA8" s="10"/>
+      <c r="BB8" s="10"/>
+      <c r="BC8" s="10"/>
+      <c r="BD8" s="10"/>
+      <c r="BE8" s="10"/>
+      <c r="BF8" s="75"/>
+      <c r="BG8" s="10"/>
+      <c r="BH8" s="10"/>
+      <c r="BI8" s="10"/>
+      <c r="BJ8" s="10"/>
+      <c r="BK8" s="10"/>
+      <c r="BL8" s="75"/>
+      <c r="BM8" s="10"/>
     </row>
     <row r="9" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="99" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="100"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="10"/>
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="10"/>
+      <c r="AH9" s="10"/>
+      <c r="AI9" s="10"/>
+      <c r="AJ9" s="10"/>
+      <c r="AK9" s="10"/>
+      <c r="AL9" s="10"/>
+      <c r="AM9" s="10"/>
+      <c r="AN9" s="10"/>
+      <c r="AO9" s="10"/>
+      <c r="AP9" s="10"/>
+      <c r="AQ9" s="10"/>
+      <c r="AR9" s="10"/>
+      <c r="AS9" s="10"/>
+      <c r="AT9" s="10"/>
+      <c r="AU9" s="10"/>
+      <c r="AV9" s="10"/>
+      <c r="AW9" s="10"/>
+      <c r="AX9" s="10"/>
+      <c r="AY9" s="75"/>
+      <c r="AZ9" s="10"/>
+      <c r="BA9" s="10"/>
+      <c r="BB9" s="10"/>
+      <c r="BC9" s="10"/>
+      <c r="BD9" s="10"/>
+      <c r="BE9" s="10"/>
+      <c r="BF9" s="75"/>
+      <c r="BG9" s="10"/>
+      <c r="BH9" s="10"/>
+      <c r="BI9" s="10"/>
+      <c r="BJ9" s="10"/>
+      <c r="BK9" s="10"/>
+      <c r="BL9" s="75"/>
+      <c r="BM9" s="10"/>
+    </row>
+    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B10" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="23" t="s">
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G10" s="21">
         <f>Netzplan!G9</f>
         <v>2</v>
       </c>
-      <c r="H9" s="21" t="str">
+      <c r="H10" s="21" t="str">
         <f>Netzplan!H9</f>
         <v>1</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I10" s="22">
         <f>Netzplan!I9</f>
         <v>1.5</v>
       </c>
-      <c r="J9" s="30">
+      <c r="J10" s="30">
         <f>Netzplan!J9</f>
         <v>1</v>
       </c>
-      <c r="K9" s="31">
-        <f>SUM(L9:BM9)</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="97"/>
-      <c r="M9" s="97"/>
-      <c r="N9" s="97"/>
-      <c r="O9" s="97"/>
-      <c r="P9" s="97"/>
-      <c r="Q9" s="97"/>
-      <c r="R9" s="97"/>
-      <c r="S9" s="97"/>
-      <c r="T9" s="97"/>
-      <c r="U9" s="97"/>
-      <c r="V9" s="97"/>
-      <c r="W9" s="97"/>
-      <c r="X9" s="97"/>
-      <c r="Y9" s="97"/>
-      <c r="Z9" s="97"/>
-      <c r="AA9" s="97"/>
-      <c r="AB9" s="97"/>
-      <c r="AC9" s="97"/>
-      <c r="AD9" s="96"/>
-      <c r="AE9" s="97"/>
-      <c r="AF9" s="97"/>
-      <c r="AG9" s="96"/>
-      <c r="AH9" s="97"/>
-      <c r="AI9" s="97"/>
-      <c r="AJ9" s="97"/>
-      <c r="AK9" s="97"/>
-      <c r="AL9" s="97"/>
-      <c r="AM9" s="97"/>
-      <c r="AN9" s="97"/>
-      <c r="AO9" s="97"/>
-      <c r="AP9" s="97"/>
-      <c r="AQ9" s="97"/>
-      <c r="AR9" s="97"/>
-      <c r="AS9" s="97"/>
-      <c r="AT9" s="97"/>
-      <c r="AU9" s="97"/>
-      <c r="AV9" s="97"/>
-      <c r="AW9" s="97"/>
-      <c r="AX9" s="97"/>
-      <c r="AY9" s="98"/>
-      <c r="AZ9" s="97"/>
-      <c r="BA9" s="97"/>
-      <c r="BB9" s="97"/>
-      <c r="BC9" s="97"/>
-      <c r="BD9" s="97"/>
-      <c r="BE9" s="97"/>
-      <c r="BF9" s="98"/>
-      <c r="BG9" s="97"/>
-      <c r="BH9" s="97"/>
-      <c r="BI9" s="97"/>
-      <c r="BJ9" s="97"/>
-      <c r="BK9" s="97"/>
-      <c r="BL9" s="98"/>
-      <c r="BM9" s="97"/>
-      <c r="BN9" s="99"/>
-    </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="K10" s="31">
+        <f t="shared" ref="K10:K20" si="1">SUM(L10:BM10)</f>
+        <v>1</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AC10" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="21"/>
+      <c r="AH10" s="10"/>
+      <c r="AI10" s="10"/>
+      <c r="AJ10" s="10"/>
+      <c r="AK10" s="10"/>
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="10"/>
+      <c r="AN10" s="10"/>
+      <c r="AO10" s="10"/>
+      <c r="AP10" s="10"/>
+      <c r="AQ10" s="10"/>
+      <c r="AR10" s="10"/>
+      <c r="AS10" s="10"/>
+      <c r="AT10" s="10"/>
+      <c r="AU10" s="10"/>
+      <c r="AV10" s="10"/>
+      <c r="AW10" s="10"/>
+      <c r="AX10" s="10"/>
+      <c r="AY10" s="75"/>
+      <c r="AZ10" s="10"/>
+      <c r="BA10" s="10"/>
+      <c r="BB10" s="10"/>
+      <c r="BC10" s="10"/>
+      <c r="BD10" s="10"/>
+      <c r="BE10" s="10"/>
+      <c r="BF10" s="75"/>
+      <c r="BG10" s="10"/>
+      <c r="BH10" s="10"/>
+      <c r="BI10" s="10"/>
+      <c r="BJ10" s="10"/>
+      <c r="BK10" s="10"/>
+      <c r="BL10" s="75"/>
+      <c r="BM10" s="10"/>
+    </row>
+    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B11" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="23" t="s">
+      <c r="C11" s="95"/>
+      <c r="D11" s="95"/>
+      <c r="E11" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G11" s="21">
         <f>Netzplan!G10</f>
         <v>2</v>
       </c>
-      <c r="H10" s="21" t="str">
+      <c r="H11" s="21" t="str">
         <f>Netzplan!H10</f>
         <v>1</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I11" s="22">
         <f>Netzplan!I10</f>
         <v>1.5</v>
       </c>
-      <c r="J10" s="30">
+      <c r="J11" s="30">
         <f>Netzplan!J10</f>
         <v>1</v>
       </c>
-      <c r="K10" s="31">
-        <f>SUM(L10:BM10)</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="97"/>
-      <c r="M10" s="97"/>
-      <c r="N10" s="97"/>
-      <c r="O10" s="97"/>
-      <c r="P10" s="97"/>
-      <c r="Q10" s="97"/>
-      <c r="R10" s="97"/>
-      <c r="S10" s="97"/>
-      <c r="T10" s="97"/>
-      <c r="U10" s="97"/>
-      <c r="V10" s="97"/>
-      <c r="W10" s="97"/>
-      <c r="X10" s="97"/>
-      <c r="Y10" s="97"/>
-      <c r="Z10" s="97"/>
-      <c r="AA10" s="97"/>
-      <c r="AB10" s="97"/>
-      <c r="AC10" s="97"/>
-      <c r="AD10" s="97"/>
-      <c r="AE10" s="97"/>
-      <c r="AF10" s="97"/>
-      <c r="AG10" s="97"/>
-      <c r="AH10" s="96"/>
-      <c r="AI10" s="96"/>
-      <c r="AJ10" s="97"/>
-      <c r="AK10" s="97"/>
-      <c r="AL10" s="97"/>
-      <c r="AM10" s="97"/>
-      <c r="AN10" s="97"/>
-      <c r="AO10" s="97"/>
-      <c r="AP10" s="97"/>
-      <c r="AQ10" s="97"/>
-      <c r="AR10" s="97"/>
-      <c r="AS10" s="97"/>
-      <c r="AT10" s="97"/>
-      <c r="AU10" s="97"/>
-      <c r="AV10" s="97"/>
-      <c r="AW10" s="97"/>
-      <c r="AX10" s="97"/>
-      <c r="AY10" s="98"/>
-      <c r="AZ10" s="97"/>
-      <c r="BA10" s="97"/>
-      <c r="BB10" s="97"/>
-      <c r="BC10" s="97"/>
-      <c r="BD10" s="97"/>
-      <c r="BE10" s="97"/>
-      <c r="BF10" s="98"/>
-      <c r="BG10" s="97"/>
-      <c r="BH10" s="97"/>
-      <c r="BI10" s="97"/>
-      <c r="BJ10" s="97"/>
-      <c r="BK10" s="97"/>
-      <c r="BL10" s="98"/>
-      <c r="BM10" s="97"/>
-      <c r="BN10" s="99"/>
-    </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="K11" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+      <c r="AH11" s="21"/>
+      <c r="AI11" s="21"/>
+      <c r="AJ11" s="10"/>
+      <c r="AK11" s="10"/>
+      <c r="AL11" s="10"/>
+      <c r="AM11" s="10"/>
+      <c r="AN11" s="10"/>
+      <c r="AO11" s="10"/>
+      <c r="AP11" s="10"/>
+      <c r="AQ11" s="10"/>
+      <c r="AR11" s="10"/>
+      <c r="AS11" s="10"/>
+      <c r="AT11" s="10"/>
+      <c r="AU11" s="10"/>
+      <c r="AV11" s="10"/>
+      <c r="AW11" s="10"/>
+      <c r="AX11" s="10"/>
+      <c r="AY11" s="75"/>
+      <c r="AZ11" s="10"/>
+      <c r="BA11" s="10"/>
+      <c r="BB11" s="10"/>
+      <c r="BC11" s="10"/>
+      <c r="BD11" s="10"/>
+      <c r="BE11" s="10"/>
+      <c r="BF11" s="75"/>
+      <c r="BG11" s="10"/>
+      <c r="BH11" s="10"/>
+      <c r="BI11" s="10"/>
+      <c r="BJ11" s="10"/>
+      <c r="BK11" s="10"/>
+      <c r="BL11" s="75"/>
+      <c r="BM11" s="10"/>
+    </row>
+    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B12" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="23" t="s">
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F12" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G12" s="21">
         <f>Netzplan!G11</f>
         <v>2</v>
       </c>
-      <c r="H11" s="21" t="str">
+      <c r="H12" s="21" t="str">
         <f>Netzplan!H11</f>
         <v>1</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I12" s="22">
         <f>Netzplan!I11</f>
         <v>1.5</v>
       </c>
-      <c r="J11" s="30">
+      <c r="J12" s="30">
         <f>Netzplan!J11</f>
         <v>1</v>
       </c>
-      <c r="K11" s="31">
-        <f>SUM(L11:BM11)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="97"/>
-      <c r="M11" s="97"/>
-      <c r="N11" s="97"/>
-      <c r="O11" s="97"/>
-      <c r="P11" s="97"/>
-      <c r="Q11" s="97"/>
-      <c r="R11" s="97"/>
-      <c r="S11" s="97"/>
-      <c r="T11" s="97"/>
-      <c r="U11" s="97"/>
-      <c r="V11" s="97"/>
-      <c r="W11" s="97"/>
-      <c r="X11" s="97"/>
-      <c r="Y11" s="97"/>
-      <c r="Z11" s="97"/>
-      <c r="AA11" s="97"/>
-      <c r="AB11" s="97"/>
-      <c r="AC11" s="97"/>
-      <c r="AD11" s="97"/>
-      <c r="AE11" s="97"/>
-      <c r="AF11" s="97"/>
-      <c r="AG11" s="97"/>
-      <c r="AH11" s="97"/>
-      <c r="AI11" s="99"/>
-      <c r="AJ11" s="96"/>
-      <c r="AK11" s="96"/>
-      <c r="AL11" s="97"/>
-      <c r="AM11" s="97"/>
-      <c r="AN11" s="97"/>
-      <c r="AO11" s="97"/>
-      <c r="AP11" s="97"/>
-      <c r="AQ11" s="97"/>
-      <c r="AR11" s="97"/>
-      <c r="AS11" s="97"/>
-      <c r="AT11" s="97"/>
-      <c r="AU11" s="97"/>
-      <c r="AV11" s="97"/>
-      <c r="AW11" s="97"/>
-      <c r="AX11" s="97"/>
-      <c r="AY11" s="98"/>
-      <c r="AZ11" s="97"/>
-      <c r="BA11" s="97"/>
-      <c r="BB11" s="97"/>
-      <c r="BC11" s="97"/>
-      <c r="BD11" s="97"/>
-      <c r="BE11" s="97"/>
-      <c r="BF11" s="98"/>
-      <c r="BG11" s="97"/>
-      <c r="BH11" s="97"/>
-      <c r="BI11" s="97"/>
-      <c r="BJ11" s="97"/>
-      <c r="BK11" s="97"/>
-      <c r="BL11" s="98"/>
-      <c r="BM11" s="97"/>
-      <c r="BN11" s="99"/>
-    </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="K12" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="10"/>
+      <c r="AJ12" s="21"/>
+      <c r="AK12" s="21"/>
+      <c r="AL12" s="10"/>
+      <c r="AM12" s="10"/>
+      <c r="AN12" s="10"/>
+      <c r="AO12" s="10"/>
+      <c r="AP12" s="10"/>
+      <c r="AQ12" s="10"/>
+      <c r="AR12" s="10"/>
+      <c r="AS12" s="10"/>
+      <c r="AT12" s="10"/>
+      <c r="AU12" s="10"/>
+      <c r="AV12" s="10"/>
+      <c r="AW12" s="10"/>
+      <c r="AX12" s="10"/>
+      <c r="AY12" s="75"/>
+      <c r="AZ12" s="10"/>
+      <c r="BA12" s="10"/>
+      <c r="BB12" s="10"/>
+      <c r="BC12" s="10"/>
+      <c r="BD12" s="10"/>
+      <c r="BE12" s="10"/>
+      <c r="BF12" s="75"/>
+      <c r="BG12" s="10"/>
+      <c r="BH12" s="10"/>
+      <c r="BI12" s="10"/>
+      <c r="BJ12" s="10"/>
+      <c r="BK12" s="10"/>
+      <c r="BL12" s="75"/>
+      <c r="BM12" s="10"/>
+    </row>
+    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="75" t="s">
+      <c r="B13" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="23" t="s">
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G13" s="21">
         <f>Netzplan!G12</f>
         <v>10</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H13" s="21">
         <f>Netzplan!H12</f>
         <v>1</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I13" s="22">
         <f>Netzplan!I12</f>
         <v>0.5</v>
       </c>
-      <c r="J12" s="30">
+      <c r="J13" s="30">
         <f>Netzplan!J12</f>
         <v>20</v>
       </c>
-      <c r="K12" s="31">
-        <f>SUM(L12:BM12)</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="97"/>
-      <c r="M12" s="97"/>
-      <c r="N12" s="97"/>
-      <c r="O12" s="97"/>
-      <c r="P12" s="97"/>
-      <c r="Q12" s="97"/>
-      <c r="R12" s="97"/>
-      <c r="S12" s="97"/>
-      <c r="T12" s="97"/>
-      <c r="U12" s="97"/>
-      <c r="V12" s="97"/>
-      <c r="W12" s="96"/>
-      <c r="X12" s="97"/>
-      <c r="Y12" s="97"/>
-      <c r="Z12" s="96"/>
-      <c r="AA12" s="96"/>
-      <c r="AB12" s="96"/>
-      <c r="AC12" s="96"/>
-      <c r="AD12" s="96"/>
-      <c r="AE12" s="97"/>
-      <c r="AF12" s="97"/>
-      <c r="AG12" s="96"/>
-      <c r="AH12" s="96"/>
-      <c r="AI12" s="96"/>
-      <c r="AJ12" s="96"/>
-      <c r="AK12" s="96"/>
-      <c r="AL12" s="97"/>
-      <c r="AM12" s="97"/>
-      <c r="AN12" s="96"/>
-      <c r="AO12" s="96"/>
-      <c r="AP12" s="96"/>
-      <c r="AQ12" s="96"/>
-      <c r="AR12" s="96"/>
-      <c r="AS12" s="97"/>
-      <c r="AT12" s="97"/>
-      <c r="AU12" s="96"/>
-      <c r="AV12" s="96"/>
-      <c r="AW12" s="96"/>
-      <c r="AX12" s="96"/>
-      <c r="AY12" s="98"/>
-      <c r="AZ12" s="97"/>
-      <c r="BA12" s="97"/>
-      <c r="BB12" s="97"/>
-      <c r="BC12" s="97"/>
-      <c r="BD12" s="97"/>
-      <c r="BE12" s="97"/>
-      <c r="BF12" s="98"/>
-      <c r="BG12" s="97"/>
-      <c r="BH12" s="97"/>
-      <c r="BI12" s="99"/>
-      <c r="BJ12" s="97"/>
-      <c r="BK12" s="97"/>
-      <c r="BL12" s="98"/>
-      <c r="BM12" s="97"/>
-      <c r="BN12" s="99"/>
-    </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="K13" s="31">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10">
+        <v>1</v>
+      </c>
+      <c r="V13" s="10">
+        <v>1</v>
+      </c>
+      <c r="W13" s="21">
+        <v>1</v>
+      </c>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="21"/>
+      <c r="AI13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="10"/>
+      <c r="AM13" s="10"/>
+      <c r="AN13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AO13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AQ13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AR13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AS13" s="10"/>
+      <c r="AT13" s="10"/>
+      <c r="AU13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AV13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AW13" s="21">
+        <v>1</v>
+      </c>
+      <c r="AX13" s="21"/>
+      <c r="AY13" s="75"/>
+      <c r="AZ13" s="10"/>
+      <c r="BA13" s="10"/>
+      <c r="BB13" s="10"/>
+      <c r="BC13" s="10"/>
+      <c r="BD13" s="10"/>
+      <c r="BE13" s="10"/>
+      <c r="BF13" s="75"/>
+      <c r="BG13" s="10"/>
+      <c r="BH13" s="10"/>
+      <c r="BJ13" s="10"/>
+      <c r="BK13" s="10"/>
+      <c r="BL13" s="75"/>
+      <c r="BM13" s="10"/>
+    </row>
+    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="75" t="s">
+      <c r="B14" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="23" t="s">
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F14" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G14" s="21">
         <f>Netzplan!G13</f>
         <v>3</v>
       </c>
-      <c r="H13" s="21" t="str">
+      <c r="H14" s="21" t="str">
         <f>Netzplan!H13</f>
         <v>1</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I14" s="22">
         <f>Netzplan!I13</f>
         <v>1.5</v>
       </c>
-      <c r="J13" s="30">
+      <c r="J14" s="30">
         <f>Netzplan!J13</f>
         <v>2</v>
       </c>
-      <c r="K13" s="31">
-        <f>SUM(L13:BM13)</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="97"/>
-      <c r="M13" s="97"/>
-      <c r="N13" s="97"/>
-      <c r="O13" s="97"/>
-      <c r="P13" s="97"/>
-      <c r="Q13" s="97"/>
-      <c r="R13" s="97"/>
-      <c r="S13" s="97"/>
-      <c r="T13" s="97"/>
-      <c r="U13" s="97"/>
-      <c r="V13" s="97"/>
-      <c r="W13" s="97"/>
-      <c r="X13" s="97"/>
-      <c r="Y13" s="97"/>
-      <c r="Z13" s="97"/>
-      <c r="AA13" s="97"/>
-      <c r="AB13" s="97"/>
-      <c r="AC13" s="97"/>
-      <c r="AD13" s="97"/>
-      <c r="AE13" s="97"/>
-      <c r="AF13" s="97"/>
-      <c r="AG13" s="97"/>
-      <c r="AH13" s="97"/>
-      <c r="AI13" s="97"/>
-      <c r="AJ13" s="97"/>
-      <c r="AK13" s="99"/>
-      <c r="AL13" s="97"/>
-      <c r="AM13" s="97"/>
-      <c r="AN13" s="96"/>
-      <c r="AO13" s="96"/>
-      <c r="AP13" s="96"/>
-      <c r="AQ13" s="97"/>
-      <c r="AR13" s="97"/>
-      <c r="AS13" s="97"/>
-      <c r="AT13" s="97"/>
-      <c r="AU13" s="97"/>
-      <c r="AV13" s="97"/>
-      <c r="AW13" s="97"/>
-      <c r="AX13" s="97"/>
-      <c r="AY13" s="98"/>
-      <c r="AZ13" s="97"/>
-      <c r="BA13" s="97"/>
-      <c r="BB13" s="97"/>
-      <c r="BC13" s="97"/>
-      <c r="BD13" s="97"/>
-      <c r="BE13" s="97"/>
-      <c r="BF13" s="98"/>
-      <c r="BG13" s="97"/>
-      <c r="BH13" s="97"/>
-      <c r="BI13" s="97"/>
-      <c r="BJ13" s="97"/>
-      <c r="BK13" s="97"/>
-      <c r="BL13" s="98"/>
-      <c r="BM13" s="97"/>
-      <c r="BN13" s="99"/>
-    </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="K14" s="31">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="10"/>
+      <c r="AE14" s="10"/>
+      <c r="AF14" s="10"/>
+      <c r="AG14" s="10"/>
+      <c r="AH14" s="10"/>
+      <c r="AI14" s="10">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="10">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="10"/>
+      <c r="AM14" s="10"/>
+      <c r="AN14" s="21"/>
+      <c r="AO14" s="21"/>
+      <c r="AP14" s="21"/>
+      <c r="AQ14" s="10"/>
+      <c r="AR14" s="10"/>
+      <c r="AS14" s="10"/>
+      <c r="AT14" s="10"/>
+      <c r="AU14" s="10"/>
+      <c r="AV14" s="10"/>
+      <c r="AW14" s="10"/>
+      <c r="AX14" s="10"/>
+      <c r="AY14" s="75"/>
+      <c r="AZ14" s="10"/>
+      <c r="BA14" s="10"/>
+      <c r="BB14" s="10"/>
+      <c r="BC14" s="10"/>
+      <c r="BD14" s="10"/>
+      <c r="BE14" s="10"/>
+      <c r="BF14" s="75"/>
+      <c r="BG14" s="10"/>
+      <c r="BH14" s="10"/>
+      <c r="BI14" s="10"/>
+      <c r="BJ14" s="10"/>
+      <c r="BK14" s="10"/>
+      <c r="BL14" s="75"/>
+      <c r="BM14" s="10"/>
+    </row>
+    <row r="15" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="75" t="s">
+      <c r="B15" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="23" t="s">
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F15" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G15" s="21">
         <f>Netzplan!G14</f>
         <v>3</v>
       </c>
-      <c r="H14" s="21" t="str">
+      <c r="H15" s="21" t="str">
         <f>Netzplan!H14</f>
         <v>1</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I15" s="22">
         <f>Netzplan!I14</f>
         <v>1.5</v>
       </c>
-      <c r="J14" s="30">
+      <c r="J15" s="30">
         <f>Netzplan!J14</f>
         <v>2</v>
       </c>
-      <c r="K14" s="31">
-        <f>SUM(L14:BM14)</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="97"/>
-      <c r="M14" s="97"/>
-      <c r="N14" s="97"/>
-      <c r="O14" s="97"/>
-      <c r="P14" s="97"/>
-      <c r="Q14" s="97"/>
-      <c r="R14" s="97"/>
-      <c r="S14" s="97"/>
-      <c r="T14" s="97"/>
-      <c r="U14" s="97"/>
-      <c r="V14" s="97"/>
-      <c r="W14" s="97"/>
-      <c r="X14" s="97"/>
-      <c r="Y14" s="97"/>
-      <c r="Z14" s="97"/>
-      <c r="AA14" s="97"/>
-      <c r="AB14" s="97"/>
-      <c r="AC14" s="97"/>
-      <c r="AD14" s="97"/>
-      <c r="AE14" s="97"/>
-      <c r="AF14" s="97"/>
-      <c r="AG14" s="97"/>
-      <c r="AH14" s="97"/>
-      <c r="AI14" s="97"/>
-      <c r="AJ14" s="97"/>
-      <c r="AK14" s="97"/>
-      <c r="AL14" s="97"/>
-      <c r="AM14" s="97"/>
-      <c r="AN14" s="97"/>
-      <c r="AO14" s="97"/>
-      <c r="AP14" s="99"/>
-      <c r="AQ14" s="96"/>
-      <c r="AR14" s="96"/>
-      <c r="AS14" s="97"/>
-      <c r="AT14" s="97"/>
-      <c r="AU14" s="96"/>
-      <c r="AV14" s="97"/>
-      <c r="AW14" s="97"/>
-      <c r="AX14" s="97"/>
-      <c r="AY14" s="98"/>
-      <c r="AZ14" s="97"/>
-      <c r="BA14" s="97"/>
-      <c r="BB14" s="97"/>
-      <c r="BC14" s="97"/>
-      <c r="BD14" s="97"/>
-      <c r="BE14" s="97"/>
-      <c r="BF14" s="98"/>
-      <c r="BG14" s="97"/>
-      <c r="BH14" s="97"/>
-      <c r="BI14" s="97"/>
-      <c r="BJ14" s="97"/>
-      <c r="BK14" s="97"/>
-      <c r="BL14" s="98"/>
-      <c r="BM14" s="97"/>
-      <c r="BN14" s="99"/>
-    </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="K15" s="31">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="10"/>
+      <c r="AF15" s="10"/>
+      <c r="AG15" s="10"/>
+      <c r="AH15" s="10"/>
+      <c r="AI15" s="10"/>
+      <c r="AJ15" s="10"/>
+      <c r="AK15" s="10">
+        <v>1</v>
+      </c>
+      <c r="AL15" s="10"/>
+      <c r="AM15" s="10"/>
+      <c r="AN15" s="10">
+        <v>1</v>
+      </c>
+      <c r="AO15" s="10"/>
+      <c r="AQ15" s="21"/>
+      <c r="AR15" s="21"/>
+      <c r="AS15" s="10"/>
+      <c r="AT15" s="10"/>
+      <c r="AU15" s="21"/>
+      <c r="AV15" s="10"/>
+      <c r="AW15" s="10"/>
+      <c r="AX15" s="10"/>
+      <c r="AY15" s="75"/>
+      <c r="AZ15" s="10"/>
+      <c r="BA15" s="10"/>
+      <c r="BB15" s="10"/>
+      <c r="BC15" s="10"/>
+      <c r="BD15" s="10"/>
+      <c r="BE15" s="10"/>
+      <c r="BF15" s="75"/>
+      <c r="BG15" s="10"/>
+      <c r="BH15" s="10"/>
+      <c r="BI15" s="10"/>
+      <c r="BJ15" s="10"/>
+      <c r="BK15" s="10"/>
+      <c r="BL15" s="75"/>
+      <c r="BM15" s="10"/>
+    </row>
+    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="10"/>
+      <c r="AD16" s="10"/>
+      <c r="AE16" s="10"/>
+      <c r="AF16" s="10"/>
+      <c r="AG16" s="10"/>
+      <c r="AH16" s="10"/>
+      <c r="AI16" s="10"/>
+      <c r="AJ16" s="10"/>
+      <c r="AK16" s="10"/>
+      <c r="AL16" s="10"/>
+      <c r="AM16" s="10"/>
+      <c r="AN16" s="10"/>
+      <c r="AQ16" s="21"/>
+      <c r="AS16" s="10"/>
+      <c r="AT16" s="10"/>
+      <c r="AU16" s="21"/>
+      <c r="AV16" s="10"/>
+      <c r="AW16" s="10"/>
+      <c r="AX16" s="10"/>
+      <c r="AY16" s="75"/>
+      <c r="AZ16" s="10"/>
+      <c r="BA16" s="10"/>
+      <c r="BB16" s="10"/>
+      <c r="BC16" s="10"/>
+      <c r="BD16" s="10"/>
+      <c r="BE16" s="10"/>
+      <c r="BF16" s="75"/>
+      <c r="BG16" s="10"/>
+      <c r="BH16" s="10"/>
+      <c r="BI16" s="10"/>
+      <c r="BJ16" s="10"/>
+      <c r="BK16" s="10"/>
+      <c r="BL16" s="75"/>
+      <c r="BM16" s="10"/>
+    </row>
+    <row r="17" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B17" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="23" t="s">
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F17" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G17" s="21">
         <f>Netzplan!G15</f>
         <v>1</v>
       </c>
-      <c r="H15" s="21" t="str">
+      <c r="H17" s="21" t="str">
         <f>Netzplan!H15</f>
         <v>1</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I17" s="22">
         <f>Netzplan!I15</f>
         <v>1.5</v>
       </c>
-      <c r="J15" s="30">
+      <c r="J17" s="30">
         <f>Netzplan!J15</f>
         <v>1</v>
       </c>
-      <c r="K15" s="31">
-        <f>SUM(L15:BM15)</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="97"/>
-      <c r="O15" s="97"/>
-      <c r="P15" s="97"/>
-      <c r="Q15" s="97"/>
-      <c r="R15" s="97"/>
-      <c r="S15" s="97"/>
-      <c r="T15" s="97"/>
-      <c r="U15" s="97"/>
-      <c r="V15" s="97"/>
-      <c r="W15" s="97"/>
-      <c r="X15" s="97"/>
-      <c r="Y15" s="97"/>
-      <c r="Z15" s="97"/>
-      <c r="AA15" s="97"/>
-      <c r="AB15" s="97"/>
-      <c r="AC15" s="97"/>
-      <c r="AD15" s="97"/>
-      <c r="AE15" s="97"/>
-      <c r="AF15" s="97"/>
-      <c r="AG15" s="97"/>
-      <c r="AH15" s="97"/>
-      <c r="AI15" s="97"/>
-      <c r="AJ15" s="97"/>
-      <c r="AK15" s="97"/>
-      <c r="AL15" s="97"/>
-      <c r="AM15" s="97"/>
-      <c r="AN15" s="97"/>
-      <c r="AO15" s="97"/>
-      <c r="AP15" s="97"/>
-      <c r="AQ15" s="97"/>
-      <c r="AR15" s="97"/>
-      <c r="AS15" s="97"/>
-      <c r="AT15" s="97"/>
-      <c r="AU15" s="97"/>
-      <c r="AV15" s="96"/>
-      <c r="AW15" s="97"/>
-      <c r="AX15" s="97"/>
-      <c r="AY15" s="98"/>
-      <c r="AZ15" s="97"/>
-      <c r="BA15" s="97"/>
-      <c r="BB15" s="97"/>
-      <c r="BC15" s="97"/>
-      <c r="BD15" s="97"/>
-      <c r="BE15" s="97"/>
-      <c r="BF15" s="98"/>
-      <c r="BG15" s="97"/>
-      <c r="BH15" s="97"/>
-      <c r="BI15" s="97"/>
-      <c r="BJ15" s="97"/>
-      <c r="BK15" s="97"/>
-      <c r="BL15" s="98"/>
-      <c r="BM15" s="97"/>
-      <c r="BN15" s="99"/>
-    </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="K17" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="10"/>
+      <c r="AE17" s="10"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="10"/>
+      <c r="AJ17" s="10"/>
+      <c r="AK17" s="10"/>
+      <c r="AL17" s="10"/>
+      <c r="AM17" s="10"/>
+      <c r="AN17" s="10"/>
+      <c r="AP17" s="10"/>
+      <c r="AQ17" s="10"/>
+      <c r="AR17" s="10">
+        <v>1</v>
+      </c>
+      <c r="AS17" s="10"/>
+      <c r="AT17" s="10"/>
+      <c r="AU17" s="10"/>
+      <c r="AV17" s="21"/>
+      <c r="AW17" s="10"/>
+      <c r="AX17" s="10"/>
+      <c r="AY17" s="75"/>
+      <c r="AZ17" s="10"/>
+      <c r="BA17" s="10"/>
+      <c r="BB17" s="10"/>
+      <c r="BC17" s="10"/>
+      <c r="BD17" s="10"/>
+      <c r="BE17" s="10"/>
+      <c r="BF17" s="75"/>
+      <c r="BG17" s="10"/>
+      <c r="BH17" s="10"/>
+      <c r="BI17" s="10"/>
+      <c r="BJ17" s="10"/>
+      <c r="BK17" s="10"/>
+      <c r="BL17" s="75"/>
+      <c r="BM17" s="10"/>
+    </row>
+    <row r="18" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B18" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="23" t="s">
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F18" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G18" s="21">
         <f>Netzplan!G16</f>
         <v>5</v>
       </c>
-      <c r="H16" s="21" t="str">
+      <c r="H18" s="21" t="str">
         <f>Netzplan!H16</f>
         <v>1</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I18" s="22">
         <f>Netzplan!I16</f>
         <v>1.5</v>
       </c>
-      <c r="J16" s="30">
+      <c r="J18" s="30">
         <f>Netzplan!J16</f>
         <v>3</v>
       </c>
-      <c r="K16" s="31">
-        <f>SUM(L16:BM16)</f>
-        <v>0</v>
-      </c>
-      <c r="L16" s="97"/>
-      <c r="M16" s="97"/>
-      <c r="N16" s="97"/>
-      <c r="O16" s="97"/>
-      <c r="P16" s="97"/>
-      <c r="Q16" s="97"/>
-      <c r="R16" s="97"/>
-      <c r="S16" s="97"/>
-      <c r="T16" s="97"/>
-      <c r="U16" s="97"/>
-      <c r="V16" s="97"/>
-      <c r="W16" s="97"/>
-      <c r="X16" s="97"/>
-      <c r="Y16" s="97"/>
-      <c r="Z16" s="97"/>
-      <c r="AA16" s="97"/>
-      <c r="AB16" s="97"/>
-      <c r="AC16" s="97"/>
-      <c r="AD16" s="97"/>
-      <c r="AE16" s="97"/>
-      <c r="AF16" s="97"/>
-      <c r="AG16" s="97"/>
-      <c r="AH16" s="97"/>
-      <c r="AI16" s="97"/>
-      <c r="AJ16" s="97"/>
-      <c r="AK16" s="97"/>
-      <c r="AL16" s="97"/>
-      <c r="AM16" s="97"/>
-      <c r="AN16" s="97"/>
-      <c r="AO16" s="97"/>
-      <c r="AP16" s="97"/>
-      <c r="AQ16" s="97"/>
-      <c r="AR16" s="97"/>
-      <c r="AS16" s="97"/>
-      <c r="AT16" s="97"/>
-      <c r="AU16" s="97"/>
-      <c r="AV16" s="97"/>
-      <c r="AW16" s="96"/>
-      <c r="AX16" s="96"/>
-      <c r="AY16" s="98"/>
-      <c r="AZ16" s="97"/>
-      <c r="BA16" s="97"/>
-      <c r="BB16" s="96"/>
-      <c r="BC16" s="97"/>
-      <c r="BD16" s="97"/>
-      <c r="BE16" s="97"/>
-      <c r="BF16" s="98"/>
-      <c r="BG16" s="97"/>
-      <c r="BH16" s="97"/>
-      <c r="BI16" s="97"/>
-      <c r="BJ16" s="99"/>
-      <c r="BK16" s="97"/>
-      <c r="BL16" s="98"/>
-      <c r="BM16" s="97"/>
-      <c r="BN16" s="99"/>
-    </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="K18" s="31">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="10"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="10"/>
+      <c r="AD18" s="10"/>
+      <c r="AE18" s="10"/>
+      <c r="AF18" s="10"/>
+      <c r="AG18" s="10"/>
+      <c r="AH18" s="10"/>
+      <c r="AI18" s="10"/>
+      <c r="AJ18" s="10"/>
+      <c r="AK18" s="10"/>
+      <c r="AL18" s="10"/>
+      <c r="AM18" s="10"/>
+      <c r="AN18" s="10"/>
+      <c r="AO18" s="10"/>
+      <c r="AS18" s="10"/>
+      <c r="AT18" s="10"/>
+      <c r="AU18" s="10">
+        <v>1</v>
+      </c>
+      <c r="AV18" s="10">
+        <v>1</v>
+      </c>
+      <c r="AW18" s="10">
+        <v>1</v>
+      </c>
+      <c r="AX18" s="21"/>
+      <c r="AY18" s="75"/>
+      <c r="AZ18" s="10"/>
+      <c r="BA18" s="10"/>
+      <c r="BB18" s="21"/>
+      <c r="BC18" s="10"/>
+      <c r="BD18" s="10"/>
+      <c r="BE18" s="10"/>
+      <c r="BF18" s="75"/>
+      <c r="BG18" s="10"/>
+      <c r="BH18" s="10"/>
+      <c r="BI18" s="10"/>
+      <c r="BK18" s="10"/>
+      <c r="BL18" s="75"/>
+      <c r="BM18" s="10"/>
+    </row>
+    <row r="19" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="101"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="10"/>
+      <c r="AH19" s="10"/>
+      <c r="AI19" s="10"/>
+      <c r="AJ19" s="10"/>
+      <c r="AK19" s="10"/>
+      <c r="AL19" s="10"/>
+      <c r="AM19" s="10"/>
+      <c r="AN19" s="10"/>
+      <c r="AO19" s="10"/>
+      <c r="AS19" s="10"/>
+      <c r="AT19" s="10"/>
+      <c r="AU19" s="10"/>
+      <c r="AV19" s="10"/>
+      <c r="AW19" s="10"/>
+      <c r="AX19" s="21"/>
+      <c r="AY19" s="75"/>
+      <c r="AZ19" s="10"/>
+      <c r="BA19" s="10"/>
+      <c r="BB19" s="21"/>
+      <c r="BC19" s="10"/>
+      <c r="BD19" s="10"/>
+      <c r="BE19" s="10"/>
+      <c r="BF19" s="75"/>
+      <c r="BG19" s="10"/>
+      <c r="BH19" s="10"/>
+      <c r="BI19" s="10"/>
+      <c r="BK19" s="10"/>
+      <c r="BL19" s="75"/>
+      <c r="BM19" s="10"/>
+    </row>
+    <row r="20" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="76" t="s">
+      <c r="B20" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="24" t="s">
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26">
+      <c r="F20" s="25"/>
+      <c r="G20" s="26">
         <f>Netzplan!G17</f>
         <v>1</v>
       </c>
-      <c r="H17" s="26" t="str">
+      <c r="H20" s="26" t="str">
         <f>Netzplan!H17</f>
         <v>1</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I20" s="32">
         <f>Netzplan!I17</f>
         <v>1</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J20" s="33">
         <f>Netzplan!J17</f>
         <v>1</v>
       </c>
-      <c r="K17" s="31">
-        <f>SUM(L17:BM17)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="100"/>
-      <c r="M17" s="100"/>
-      <c r="N17" s="100"/>
-      <c r="O17" s="100"/>
-      <c r="P17" s="100"/>
-      <c r="Q17" s="100"/>
-      <c r="R17" s="100"/>
-      <c r="S17" s="100"/>
-      <c r="T17" s="100"/>
-      <c r="U17" s="100"/>
-      <c r="V17" s="100"/>
-      <c r="W17" s="100"/>
-      <c r="X17" s="100"/>
-      <c r="Y17" s="100"/>
-      <c r="Z17" s="100"/>
-      <c r="AA17" s="100"/>
-      <c r="AB17" s="100"/>
-      <c r="AC17" s="100"/>
-      <c r="AD17" s="100"/>
-      <c r="AE17" s="100"/>
-      <c r="AF17" s="100"/>
-      <c r="AG17" s="100"/>
-      <c r="AH17" s="100"/>
-      <c r="AI17" s="100"/>
-      <c r="AJ17" s="100"/>
-      <c r="AK17" s="100"/>
-      <c r="AL17" s="100"/>
-      <c r="AM17" s="100"/>
-      <c r="AN17" s="100"/>
-      <c r="AO17" s="100"/>
-      <c r="AP17" s="100"/>
-      <c r="AQ17" s="100"/>
-      <c r="AR17" s="100"/>
-      <c r="AS17" s="100"/>
-      <c r="AT17" s="100"/>
-      <c r="AU17" s="100"/>
-      <c r="AV17" s="100"/>
-      <c r="AW17" s="100"/>
-      <c r="AX17" s="100"/>
-      <c r="AY17" s="101"/>
-      <c r="AZ17" s="100"/>
-      <c r="BA17" s="100"/>
-      <c r="BB17" s="100"/>
-      <c r="BC17" s="96"/>
-      <c r="BD17" s="100"/>
-      <c r="BE17" s="100"/>
-      <c r="BF17" s="101"/>
-      <c r="BG17" s="100"/>
-      <c r="BH17" s="100"/>
-      <c r="BI17" s="100"/>
-      <c r="BJ17" s="100"/>
-      <c r="BK17" s="100"/>
-      <c r="BL17" s="101"/>
-      <c r="BM17" s="100"/>
-      <c r="BN17" s="99"/>
+      <c r="K20" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="12"/>
+      <c r="AA20" s="12"/>
+      <c r="AB20" s="12"/>
+      <c r="AC20" s="12"/>
+      <c r="AD20" s="12"/>
+      <c r="AE20" s="12"/>
+      <c r="AF20" s="12"/>
+      <c r="AG20" s="12"/>
+      <c r="AH20" s="12"/>
+      <c r="AI20" s="12"/>
+      <c r="AJ20" s="12"/>
+      <c r="AK20" s="12"/>
+      <c r="AL20" s="12"/>
+      <c r="AM20" s="12"/>
+      <c r="AN20" s="12"/>
+      <c r="AO20" s="12"/>
+      <c r="AP20" s="12"/>
+      <c r="AQ20" s="12"/>
+      <c r="AR20" s="12"/>
+      <c r="AS20" s="12"/>
+      <c r="AT20" s="12"/>
+      <c r="AU20" s="12"/>
+      <c r="AV20" s="12"/>
+      <c r="AW20" s="12"/>
+      <c r="AZ20" s="12"/>
+      <c r="BA20" s="12"/>
+      <c r="BB20" s="12">
+        <v>1</v>
+      </c>
+      <c r="BC20" s="21"/>
+      <c r="BD20" s="12"/>
+      <c r="BE20" s="12"/>
+      <c r="BF20" s="76"/>
+      <c r="BG20" s="12"/>
+      <c r="BH20" s="12"/>
+      <c r="BI20" s="12"/>
+      <c r="BJ20" s="12"/>
+      <c r="BK20" s="12"/>
+      <c r="BL20" s="76"/>
+      <c r="BM20" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="20">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:K17">
-    <cfRule type="expression" dxfId="7" priority="5">
+  <conditionalFormatting sqref="K2:K20">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>IF(K2&lt;&gt;J2,TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:BM17">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>IF(OR(WEEKDAY(M$1)=7,WEEKDAY(M$1)=1),1,0)</formula>
+  <conditionalFormatting sqref="L1:BM9 L10:Z11 AE10:BM11 L12:BM15 L17:AN17 AP17:AQ17 AS16:BM17 L18:AO19 AS18:AT19 AX18:BM19 L16:AM16 AP16 L20:AW20 BC20:BM20 AZ20:BA20">
+    <cfRule type="expression" dxfId="12" priority="1">
+      <formula>IF(OR(WEEKDAY(L$1)=7,WEEKDAY(L$1)=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:BM17">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+  <conditionalFormatting sqref="L2:BM9 L10:Z11 AC10:BM11 L12:BM15 AS16:BM16 AP17:BM17 L18:AO19 AS18:BM19 AP16:AQ16 L16:AN17 L20:AW20 AZ20:BM20">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC10:AD11">
+    <cfRule type="expression" dxfId="9" priority="20">
+      <formula>IF(OR(WEEKDAY(AA$1)=7,WEEKDAY(AA$1)=1),1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ16 AN16">
+    <cfRule type="expression" dxfId="7" priority="24">
+      <formula>IF(OR(WEEKDAY(AO$1)=7,WEEKDAY(AO$1)=1),1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR17 BB20">
+    <cfRule type="expression" dxfId="5" priority="28">
+      <formula>IF(OR(WEEKDAY(AO$1)=7,WEEKDAY(AO$1)=1),1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU18:AW19">
+    <cfRule type="expression" dxfId="3" priority="32">
+      <formula>IF(OR(WEEKDAY(AP$1)=7,WEEKDAY(AP$1)=1),1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB20">
+    <cfRule type="expression" dxfId="1" priority="36">
+      <formula>IF(OR(WEEKDAY(AX$1)=7,WEEKDAY(AX$1)=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -5678,12 +6154,13 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="3" id="{00000000-000E-0000-0200-000002000000}">
-            <xm:f>ISNUMBER(_xlfn.XMATCH(M$1,FeiertageMV!$A$1:$A$30,0))</xm:f>
+            <xm:f>ISNUMBER(_xlfn.XMATCH(L$1,FeiertageMV!$A$1:$A$30,0))</xm:f>
             <x14:dxf>
               <font>
                 <color theme="0"/>
@@ -5698,7 +6175,102 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>L1:BM17</xm:sqref>
+          <xm:sqref>L1:BM9 L10:Z11 AE10:BM11 L12:BM15 L17:AN17 AP17:AQ17 AS16:BM17 L18:AO19 AS18:AT19 AX18:BM19 L16:AM16 AP16 L20:AW20 BC20:BM20 AZ20:BA20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="21" id="{00000000-000E-0000-0200-000002000000}">
+            <xm:f>ISNUMBER(_xlfn.XMATCH(AA$1,FeiertageMV!$A$1:$A$30,0))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="0"/>
+                <name val="Arial"/>
+                <family val="2"/>
+                <charset val="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF7030A0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AC10:AD11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="25" id="{00000000-000E-0000-0200-000002000000}">
+            <xm:f>ISNUMBER(_xlfn.XMATCH(AO$1,FeiertageMV!$A$1:$A$30,0))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="0"/>
+                <name val="Arial"/>
+                <family val="2"/>
+                <charset val="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF7030A0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AQ16 AN16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="29" id="{00000000-000E-0000-0200-000002000000}">
+            <xm:f>ISNUMBER(_xlfn.XMATCH(AO$1,FeiertageMV!$A$1:$A$30,0))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="0"/>
+                <name val="Arial"/>
+                <family val="2"/>
+                <charset val="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF7030A0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AR17 BB20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="33" id="{00000000-000E-0000-0200-000002000000}">
+            <xm:f>ISNUMBER(_xlfn.XMATCH(AP$1,FeiertageMV!$A$1:$A$30,0))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="0"/>
+                <name val="Arial"/>
+                <family val="2"/>
+                <charset val="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF7030A0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>AU18:AW19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="37" id="{00000000-000E-0000-0200-000002000000}">
+            <xm:f>ISNUMBER(_xlfn.XMATCH(AX$1,FeiertageMV!$A$1:$A$30,0))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="0"/>
+                <name val="Arial"/>
+                <family val="2"/>
+                <charset val="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF7030A0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>BB20</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5716,11 +6288,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="102" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" style="77" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="77" t="s">
         <v>73</v>
       </c>
       <c r="B1" t="s">
@@ -5728,7 +6300,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="102">
+      <c r="A2" s="77">
         <v>44927</v>
       </c>
       <c r="B2" t="s">
@@ -5736,7 +6308,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="102">
+      <c r="A3" s="77">
         <v>45022</v>
       </c>
       <c r="B3" t="s">
@@ -5744,7 +6316,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="102">
+      <c r="A4" s="77">
         <v>45023</v>
       </c>
       <c r="B4" t="s">
@@ -5752,7 +6324,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="102">
+      <c r="A5" s="77">
         <v>45025</v>
       </c>
       <c r="B5" t="s">
@@ -5760,7 +6332,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="102">
+      <c r="A6" s="77">
         <v>45026</v>
       </c>
       <c r="B6" t="s">
@@ -5768,7 +6340,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="102">
+      <c r="A7" s="77">
         <v>45047</v>
       </c>
       <c r="B7" t="s">
@@ -5776,7 +6348,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="102">
+      <c r="A8" s="77">
         <v>45071</v>
       </c>
       <c r="B8" t="s">
@@ -5784,7 +6356,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="102">
+      <c r="A9" s="77">
         <v>45081</v>
       </c>
       <c r="B9" t="s">
@@ -5792,7 +6364,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="102">
+      <c r="A10" s="77">
         <v>45082</v>
       </c>
       <c r="B10" t="s">
@@ -5800,7 +6372,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="102">
+      <c r="A11" s="77">
         <v>45202</v>
       </c>
       <c r="B11" t="s">
@@ -5808,7 +6380,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="102">
+      <c r="A12" s="77">
         <v>45230</v>
       </c>
       <c r="B12" t="s">
@@ -5816,7 +6388,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="102">
+      <c r="A13" s="77">
         <v>45285</v>
       </c>
       <c r="B13" t="s">
@@ -5824,7 +6396,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="102">
+      <c r="A14" s="77">
         <v>45286</v>
       </c>
       <c r="B14" t="s">

</xml_diff>